<commit_message>
added facts rewriting of dataset
</commit_message>
<xml_diff>
--- a/Dataset/MappingConDatiArticolo.xlsx
+++ b/Dataset/MappingConDatiArticolo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Documents/OttimizzazioneEnergetica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/PycharmProjects/EnergyOptimization/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1105676-41ED-5E4D-9F56-4A16AE2F6A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4FD0F4-EABB-4445-909C-441761176180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{ADBE4949-0076-D64E-ACAC-FDF7396AF500}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{ADBE4949-0076-D64E-ACAC-FDF7396AF500}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t> Discharge(Wh)</t>
   </si>
@@ -83,27 +83,12 @@
     <t>EStd</t>
   </si>
   <si>
-    <t>Pgtd (se &gt; 0)</t>
-  </si>
-  <si>
-    <t>Pgtd (se &lt; 0)</t>
-  </si>
-  <si>
     <t> Feed-in(W)</t>
   </si>
   <si>
     <t> From grid(W)</t>
   </si>
   <si>
-    <t>Pgtd = Egtd / t (se &lt; 0)</t>
-  </si>
-  <si>
-    <t>Pgtd = Egtd / t(se &gt; 0)</t>
-  </si>
-  <si>
-    <t>Estd / t</t>
-  </si>
-  <si>
     <t>PStd (se &gt; 0)</t>
   </si>
   <si>
@@ -120,13 +105,49 @@
   </si>
   <si>
     <t>vP_S_d</t>
+  </si>
+  <si>
+    <t>Pgtd = Egtd / 60 (se &lt; 0, 60 perché è un minuto)</t>
+  </si>
+  <si>
+    <t>Pgtd = Egtd / 60 (se &gt; 0, 60 perché è un minuto)</t>
+  </si>
+  <si>
+    <t>Egtd (se &lt; 0)</t>
+  </si>
+  <si>
+    <t>Egtd (se &gt; 0)</t>
+  </si>
+  <si>
+    <t>Estd / 60 (60 perché è un minuto)</t>
+  </si>
+  <si>
+    <t>Energia</t>
+  </si>
+  <si>
+    <t>Potenza</t>
+  </si>
+  <si>
+    <t>Dataset Articolo</t>
+  </si>
+  <si>
+    <t>Mapping Modello semplificato</t>
+  </si>
+  <si>
+    <t>Mapping predicati ASP</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +174,13 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,11 +202,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -513,121 +545,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FB51B3-BC7A-C147-8BBC-2B18BA296EF7}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>11</v>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>